<commit_message>
added link for further research
</commit_message>
<xml_diff>
--- a/MTG/DeckWishList.xlsx
+++ b/MTG/DeckWishList.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$1</definedName>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
   <si>
     <t>Talent of the Telepath</t>
   </si>
@@ -131,6 +132,9 @@
   </si>
   <si>
     <t>Card</t>
+  </si>
+  <si>
+    <t>http://gatherer.wizards.com/Pages/Search/Default.aspx?action=advanced&amp;color=+![W]+![B]+![R]+![G]&amp;text=+[creatures]+[you]+[control]</t>
   </si>
 </sst>
 </file>
@@ -451,9 +455,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,4 +649,22 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>